<commit_message>
text file containing tasklist
</commit_message>
<xml_diff>
--- a/mapMockUp.xlsx
+++ b/mapMockUp.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etsai\Documents\GitHub\robot_planning\final project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etsai\Documents\GitHub\robot_planning_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9485CCD-3C98-4AC3-AA88-A1A79843E6A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929A66BC-268C-4700-96CE-8513B9CA196E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{1517CA63-02F6-499E-8C90-A9137DCB2EA7}"/>
+    <workbookView xWindow="14235" yWindow="2745" windowWidth="14400" windowHeight="7375" xr2:uid="{1517CA63-02F6-499E-8C90-A9137DCB2EA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
   <si>
     <t>Supply A</t>
   </si>
@@ -399,7 +399,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -419,9 +419,6 @@
       <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C5" t="s">

</xml_diff>

<commit_message>
need to fix A* can only be called once
probably something to with global variables
</commit_message>
<xml_diff>
--- a/mapMockUp.xlsx
+++ b/mapMockUp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\etsai\Documents\GitHub\robot_planning_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929A66BC-268C-4700-96CE-8513B9CA196E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488A3F91-0615-460E-A0C9-31F23E3C7FB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14235" yWindow="2745" windowWidth="14400" windowHeight="7375" xr2:uid="{1517CA63-02F6-499E-8C90-A9137DCB2EA7}"/>
   </bookViews>
@@ -60,12 +60,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,8 +86,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +406,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -408,32 +415,53 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
       <c r="H1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="E3" t="s">
         <v>2</v>
       </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="1"/>
       <c r="C5" t="s">
         <v>2</v>
       </c>
+      <c r="D5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="1"/>
       <c r="F6" t="s">
         <v>3</v>
       </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>3</v>
       </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">

</xml_diff>